<commit_message>
Diagrama de sequência atualizado assim como a apresentação
</commit_message>
<xml_diff>
--- a/Documentos/Documentos do Projeto/Estimativa de Projeto/ESTIMATIVA.xlsx
+++ b/Documentos/Documentos do Projeto/Estimativa de Projeto/ESTIMATIVA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BrenoXDMoon\Documents\GitHub\ProjetoLes\Documentos\Estimativa de Projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BrenoXDMoon\Documents\GitHub\ProjetoLes\Documentos\Documentos do Projeto\Estimativa de Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50712AC6-CB01-454A-95DD-1602E6491EF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627E451F-6AC3-4DCA-B3B3-2E9863D2A6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D9FF7230-91BA-A544-8A5A-3054F2DD43A9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="79">
   <si>
     <t>(horas)</t>
   </si>
@@ -204,12 +204,6 @@
   </si>
   <si>
     <t>Alterar Status do Pedido</t>
-  </si>
-  <si>
-    <t>Em Andamento</t>
-  </si>
-  <si>
-    <t>Não iniciado</t>
   </si>
   <si>
     <t>Finalizado</t>
@@ -282,7 +276,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -340,22 +334,8 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,16 +363,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -437,13 +407,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -512,30 +480,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="2">
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutro" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Ruim" xfId="3" builtinId="27"/>
   </cellStyles>
   <dxfs count="24">
     <dxf>
@@ -1096,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B692412-8401-4F44-8DDD-33476696CC96}">
   <dimension ref="A1:U72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J36"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K64" sqref="K64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1148,11 +1108,11 @@
       <c r="E2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
       <c r="I2" s="6" t="s">
         <v>9</v>
       </c>
@@ -1203,8 +1163,8 @@
         <v>3</v>
       </c>
       <c r="I4" s="21"/>
-      <c r="J4" s="25" t="s">
-        <v>59</v>
+      <c r="J4" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1227,8 +1187,8 @@
         <v>3</v>
       </c>
       <c r="I5" s="21"/>
-      <c r="J5" s="25" t="s">
-        <v>59</v>
+      <c r="J5" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -1251,8 +1211,8 @@
         <v>3</v>
       </c>
       <c r="I6" s="21"/>
-      <c r="J6" s="25" t="s">
-        <v>59</v>
+      <c r="J6" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -1275,8 +1235,8 @@
         <v>3</v>
       </c>
       <c r="I7" s="21"/>
-      <c r="J7" s="25" t="s">
-        <v>59</v>
+      <c r="J7" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -1299,8 +1259,8 @@
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="21"/>
-      <c r="J8" s="25" t="s">
-        <v>59</v>
+      <c r="J8" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -1323,8 +1283,8 @@
         <v>3</v>
       </c>
       <c r="I9" s="21"/>
-      <c r="J9" s="25" t="s">
-        <v>59</v>
+      <c r="J9" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -1347,8 +1307,8 @@
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
       <c r="I10" s="21"/>
-      <c r="J10" s="25" t="s">
-        <v>59</v>
+      <c r="J10" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -1371,8 +1331,8 @@
       </c>
       <c r="H11" s="19"/>
       <c r="I11" s="21"/>
-      <c r="J11" s="25" t="s">
-        <v>59</v>
+      <c r="J11" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -1395,8 +1355,8 @@
       </c>
       <c r="H12" s="19"/>
       <c r="I12" s="21"/>
-      <c r="J12" s="25" t="s">
-        <v>59</v>
+      <c r="J12" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -1419,8 +1379,8 @@
       </c>
       <c r="H13" s="19"/>
       <c r="I13" s="21"/>
-      <c r="J13" s="25" t="s">
-        <v>59</v>
+      <c r="J13" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -1443,8 +1403,8 @@
         <v>3</v>
       </c>
       <c r="I14" s="21"/>
-      <c r="J14" s="25" t="s">
-        <v>59</v>
+      <c r="J14" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -1467,8 +1427,8 @@
         <v>3</v>
       </c>
       <c r="I15" s="21"/>
-      <c r="J15" s="25" t="s">
-        <v>59</v>
+      <c r="J15" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -1491,8 +1451,8 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="21"/>
-      <c r="J16" s="25" t="s">
-        <v>59</v>
+      <c r="J16" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1515,14 +1475,14 @@
         <v>3</v>
       </c>
       <c r="I17" s="21"/>
-      <c r="J17" s="25" t="s">
-        <v>59</v>
+      <c r="J17" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C18" s="19">
         <v>2</v>
@@ -1539,7 +1499,7 @@
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
       <c r="I18" s="21"/>
-      <c r="J18" s="25"/>
+      <c r="J18" s="24"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="20"/>
@@ -1561,8 +1521,8 @@
         <v>3</v>
       </c>
       <c r="I19" s="21"/>
-      <c r="J19" s="25" t="s">
-        <v>59</v>
+      <c r="J19" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1585,8 +1545,8 @@
         <v>3</v>
       </c>
       <c r="I20" s="21"/>
-      <c r="J20" s="25" t="s">
-        <v>59</v>
+      <c r="J20" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1633,8 +1593,8 @@
       </c>
       <c r="H22" s="19"/>
       <c r="I22" s="21"/>
-      <c r="J22" s="27" t="s">
-        <v>58</v>
+      <c r="J22" s="24" t="s">
+        <v>57</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>46</v>
@@ -1660,8 +1620,8 @@
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
       <c r="I23" s="21"/>
-      <c r="J23" s="27" t="s">
-        <v>58</v>
+      <c r="J23" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1684,8 +1644,8 @@
         <v>3</v>
       </c>
       <c r="I24" s="21"/>
-      <c r="J24" s="27" t="s">
-        <v>58</v>
+      <c r="J24" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1708,8 +1668,8 @@
         <v>3</v>
       </c>
       <c r="I25" s="21"/>
-      <c r="J25" s="27" t="s">
-        <v>58</v>
+      <c r="J25" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1732,8 +1692,8 @@
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
       <c r="I26" s="21"/>
-      <c r="J26" s="27" t="s">
-        <v>58</v>
+      <c r="J26" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1756,8 +1716,8 @@
       </c>
       <c r="H27" s="19"/>
       <c r="I27" s="21"/>
-      <c r="J27" s="27" t="s">
-        <v>58</v>
+      <c r="J27" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1780,8 +1740,8 @@
       <c r="G28" s="19"/>
       <c r="H28" s="19"/>
       <c r="I28" s="21"/>
-      <c r="J28" s="27" t="s">
-        <v>58</v>
+      <c r="J28" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1804,8 +1764,8 @@
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
       <c r="I29" s="21"/>
-      <c r="J29" s="27" t="s">
-        <v>58</v>
+      <c r="J29" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -1828,8 +1788,8 @@
       </c>
       <c r="H30" s="19"/>
       <c r="I30" s="21"/>
-      <c r="J30" s="27" t="s">
-        <v>58</v>
+      <c r="J30" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1852,8 +1812,8 @@
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
       <c r="I31" s="21"/>
-      <c r="J31" s="27" t="s">
-        <v>58</v>
+      <c r="J31" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1876,8 +1836,8 @@
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
       <c r="I32" s="21"/>
-      <c r="J32" s="27" t="s">
-        <v>58</v>
+      <c r="J32" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
@@ -1900,8 +1860,8 @@
         <v>3</v>
       </c>
       <c r="I33" s="21"/>
-      <c r="J33" s="27" t="s">
-        <v>58</v>
+      <c r="J33" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -1924,8 +1884,8 @@
         <v>3</v>
       </c>
       <c r="I34" s="21"/>
-      <c r="J34" s="27" t="s">
-        <v>58</v>
+      <c r="J34" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -1948,8 +1908,8 @@
       </c>
       <c r="H35" s="19"/>
       <c r="I35" s="21"/>
-      <c r="J35" s="27" t="s">
-        <v>58</v>
+      <c r="J35" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -1972,8 +1932,8 @@
       </c>
       <c r="H36" s="19"/>
       <c r="I36" s="21"/>
-      <c r="J36" s="27" t="s">
-        <v>58</v>
+      <c r="J36" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1987,7 +1947,7 @@
       <c r="D37" s="19">
         <v>7</v>
       </c>
-      <c r="E37" s="29">
+      <c r="E37" s="26">
         <v>13</v>
       </c>
       <c r="F37" s="19" t="s">
@@ -1996,8 +1956,8 @@
       <c r="G37" s="19"/>
       <c r="H37" s="19"/>
       <c r="I37" s="21"/>
-      <c r="J37" s="27" t="s">
-        <v>58</v>
+      <c r="J37" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -2034,14 +1994,14 @@
       </c>
       <c r="H39" s="19"/>
       <c r="I39" s="21"/>
-      <c r="J39" s="25" t="s">
-        <v>59</v>
+      <c r="J39" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="20"/>
       <c r="B40" s="22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C40" s="19">
         <v>2</v>
@@ -2058,16 +2018,16 @@
       </c>
       <c r="H40" s="19"/>
       <c r="I40" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="J40" s="25" t="s">
-        <v>59</v>
+        <v>74</v>
+      </c>
+      <c r="J40" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="20"/>
       <c r="B41" s="22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C41" s="19"/>
       <c r="D41" s="19"/>
@@ -2078,14 +2038,14 @@
       </c>
       <c r="H41" s="19"/>
       <c r="I41" s="21"/>
-      <c r="J41" s="25" t="s">
-        <v>59</v>
+      <c r="J41" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="20"/>
       <c r="B42" s="22" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C42" s="19">
         <v>2</v>
@@ -2102,8 +2062,8 @@
       </c>
       <c r="H42" s="19"/>
       <c r="I42" s="21"/>
-      <c r="J42" s="25" t="s">
-        <v>59</v>
+      <c r="J42" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -2126,14 +2086,14 @@
       </c>
       <c r="H43" s="19"/>
       <c r="I43" s="21"/>
-      <c r="J43" s="25" t="s">
-        <v>59</v>
+      <c r="J43" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="20"/>
       <c r="B44" s="22" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C44" s="19">
         <v>2</v>
@@ -2150,8 +2110,8 @@
       </c>
       <c r="H44" s="19"/>
       <c r="I44" s="21"/>
-      <c r="J44" s="25" t="s">
-        <v>59</v>
+      <c r="J44" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -2174,14 +2134,14 @@
       </c>
       <c r="H45" s="19"/>
       <c r="I45" s="21"/>
-      <c r="J45" s="25" t="s">
-        <v>59</v>
+      <c r="J45" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="20"/>
       <c r="B46" s="22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C46" s="19">
         <v>2</v>
@@ -2198,14 +2158,14 @@
       </c>
       <c r="H46" s="19"/>
       <c r="I46" s="21"/>
-      <c r="J46" s="25" t="s">
-        <v>59</v>
+      <c r="J46" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="20"/>
       <c r="B47" s="22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C47" s="19">
         <v>2</v>
@@ -2222,14 +2182,14 @@
       </c>
       <c r="H47" s="19"/>
       <c r="I47" s="21"/>
-      <c r="J47" s="25" t="s">
-        <v>59</v>
+      <c r="J47" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="20"/>
       <c r="B48" s="22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C48" s="19">
         <v>2</v>
@@ -2246,14 +2206,14 @@
       </c>
       <c r="H48" s="19"/>
       <c r="I48" s="21"/>
-      <c r="J48" s="25" t="s">
-        <v>59</v>
+      <c r="J48" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="20"/>
       <c r="B49" s="22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C49" s="19">
         <v>2</v>
@@ -2270,14 +2230,14 @@
       </c>
       <c r="H49" s="19"/>
       <c r="I49" s="21"/>
-      <c r="J49" s="25" t="s">
-        <v>59</v>
+      <c r="J49" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="20"/>
       <c r="B50" s="22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C50" s="19">
         <v>2</v>
@@ -2294,14 +2254,14 @@
       </c>
       <c r="H50" s="19"/>
       <c r="I50" s="21"/>
-      <c r="J50" s="25" t="s">
-        <v>59</v>
+      <c r="J50" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="20"/>
       <c r="B51" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C51" s="19">
         <v>2</v>
@@ -2318,14 +2278,14 @@
       </c>
       <c r="H51" s="19"/>
       <c r="I51" s="21"/>
-      <c r="J51" s="25" t="s">
-        <v>59</v>
+      <c r="J51" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A52" s="20"/>
       <c r="B52" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C52" s="19">
         <v>2</v>
@@ -2341,17 +2301,17 @@
         <v>2</v>
       </c>
       <c r="H52" s="19"/>
-      <c r="I52" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="J52" s="25" t="s">
-        <v>59</v>
+      <c r="I52" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="J52" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="20"/>
       <c r="B53" s="22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C53" s="19">
         <v>2</v>
@@ -2367,15 +2327,15 @@
         <v>2</v>
       </c>
       <c r="H53" s="19"/>
-      <c r="I53" s="26"/>
-      <c r="J53" s="25" t="s">
-        <v>59</v>
+      <c r="I53" s="25"/>
+      <c r="J53" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="20"/>
       <c r="B54" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C54" s="19">
         <v>2</v>
@@ -2391,15 +2351,15 @@
         <v>2</v>
       </c>
       <c r="H54" s="19"/>
-      <c r="I54" s="26"/>
-      <c r="J54" s="25" t="s">
-        <v>59</v>
+      <c r="I54" s="25"/>
+      <c r="J54" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="20"/>
       <c r="B55" s="22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C55" s="19">
         <v>2</v>
@@ -2415,15 +2375,15 @@
         <v>2</v>
       </c>
       <c r="H55" s="19"/>
-      <c r="I55" s="26"/>
-      <c r="J55" s="25" t="s">
-        <v>59</v>
+      <c r="I55" s="25"/>
+      <c r="J55" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="20"/>
       <c r="B56" s="22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C56" s="19">
         <v>2</v>
@@ -2439,17 +2399,17 @@
         <v>2</v>
       </c>
       <c r="H56" s="19"/>
-      <c r="I56" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="J56" s="25" t="s">
-        <v>59</v>
+      <c r="I56" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="J56" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="20"/>
       <c r="B57" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C57" s="19">
         <v>2</v>
@@ -2465,9 +2425,9 @@
         <v>2</v>
       </c>
       <c r="H57" s="19"/>
-      <c r="I57" s="26"/>
-      <c r="J57" s="25" t="s">
-        <v>59</v>
+      <c r="I57" s="25"/>
+      <c r="J57" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -2490,8 +2450,8 @@
       </c>
       <c r="H58" s="19"/>
       <c r="I58" s="21"/>
-      <c r="J58" s="25" t="s">
-        <v>59</v>
+      <c r="J58" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
@@ -2514,8 +2474,8 @@
       </c>
       <c r="H59" s="19"/>
       <c r="I59" s="21"/>
-      <c r="J59" s="25" t="s">
-        <v>59</v>
+      <c r="J59" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -2538,14 +2498,14 @@
       </c>
       <c r="H60" s="19"/>
       <c r="I60" s="21"/>
-      <c r="J60" s="25" t="s">
-        <v>59</v>
+      <c r="J60" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="20"/>
       <c r="B61" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C61" s="19"/>
       <c r="D61" s="19"/>
@@ -2556,8 +2516,8 @@
       </c>
       <c r="H61" s="19"/>
       <c r="I61" s="21"/>
-      <c r="J61" s="25" t="s">
-        <v>59</v>
+      <c r="J61" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -2580,8 +2540,8 @@
       </c>
       <c r="H62" s="19"/>
       <c r="I62" s="21"/>
-      <c r="J62" s="25" t="s">
-        <v>59</v>
+      <c r="J62" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
@@ -2604,8 +2564,8 @@
       </c>
       <c r="H63" s="19"/>
       <c r="I63" s="21"/>
-      <c r="J63" s="25" t="s">
-        <v>59</v>
+      <c r="J63" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -2628,8 +2588,8 @@
       </c>
       <c r="H64" s="19"/>
       <c r="I64" s="21"/>
-      <c r="J64" s="25" t="s">
-        <v>59</v>
+      <c r="J64" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
@@ -2815,23 +2775,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ReferenceId xmlns="13526e60-2309-4b29-b958-df71ed96cd48" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100301B24C317AEAA4A9E81584B0F1753BF" ma:contentTypeVersion="1" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="ea2d69a61fc7a42705a79b5983b790a2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="13526e60-2309-4b29-b958-df71ed96cd48" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0df65a6dff0c15483f5753a509519d7a" ns2:_="">
     <xsd:import namespace="13526e60-2309-4b29-b958-df71ed96cd48"/>
@@ -2957,25 +2900,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C51C229-CA01-440E-B2BE-F6F69B7DA214}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="13526e60-2309-4b29-b958-df71ed96cd48"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A55BC6FF-54C9-4DD8-8203-E7CA3890AFA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ReferenceId xmlns="13526e60-2309-4b29-b958-df71ed96cd48" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AAA58E31-EA10-4926-9E03-5E76E8F2B1AF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2991,4 +2933,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A55BC6FF-54C9-4DD8-8203-E7CA3890AFA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C51C229-CA01-440E-B2BE-F6F69B7DA214}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="13526e60-2309-4b29-b958-df71ed96cd48"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>